<commit_message>
Nueva actualización de limpieza géneros
</commit_message>
<xml_diff>
--- a/hito-2/genres_map.xlsx
+++ b/hito-2/genres_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conid\Desktop\Universidad\2025 Otoño\Mineria de Datos\Proyecto\proyecto-mineria\hito-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78893063-6938-458A-B1BC-3041A862A6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BCACAD-99C3-4F2F-B55B-134A362D2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00A398F6-67CE-47C1-A2A2-62B40E6B4FF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>role-playing</t>
   </si>
@@ -264,13 +264,55 @@
   </si>
   <si>
     <t>historical</t>
+  </si>
+  <si>
+    <t>adventure-puzzle</t>
+  </si>
+  <si>
+    <t>adventure puzzle</t>
+  </si>
+  <si>
+    <t>puzzle-platform</t>
+  </si>
+  <si>
+    <t>puzzle platform</t>
+  </si>
+  <si>
+    <t>minigames</t>
+  </si>
+  <si>
+    <t>mini-game</t>
+  </si>
+  <si>
+    <t>third-person</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> third person</t>
+  </si>
+  <si>
+    <t>massively multiplayer online role-playing game</t>
+  </si>
+  <si>
+    <t>mmorpg</t>
+  </si>
+  <si>
+    <t>turn-based strategy</t>
+  </si>
+  <si>
+    <t>tbs</t>
+  </si>
+  <si>
+    <t>real-time</t>
+  </si>
+  <si>
+    <t>real time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +325,17 @@
       <color rgb="FF6688CC"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,9 +358,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,13 +699,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B1DF5-292F-4CAE-B96E-0AC01ED929CA}">
-  <dimension ref="A2:F34"/>
+  <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="142" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
@@ -661,7 +718,7 @@
     <col min="11" max="11" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -672,18 +729,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -694,7 +751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -711,7 +768,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -719,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -737,7 +794,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -745,7 +802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -756,7 +813,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -764,7 +821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -772,7 +829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -783,7 +840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -791,7 +848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -799,15 +856,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -815,7 +872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -823,7 +880,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -834,7 +891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -842,7 +899,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -850,7 +907,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -858,7 +915,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -869,7 +926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -877,7 +934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -885,7 +942,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -893,7 +950,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -901,7 +958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -909,7 +966,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -917,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -925,15 +982,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -941,7 +998,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -949,7 +1006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -957,7 +1014,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -971,7 +1028,64 @@
         <v>75</v>
       </c>
     </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega codigo para reducir géneros
</commit_message>
<xml_diff>
--- a/hito-2/genres_map.xlsx
+++ b/hito-2/genres_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conid\Desktop\Universidad\2025 Otoño\Mineria de Datos\Proyecto\proyecto-mineria\hito-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BCACAD-99C3-4F2F-B55B-134A362D2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C952882-2936-4F8E-905D-FF998770349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00A398F6-67CE-47C1-A2A2-62B40E6B4FF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>role-playing</t>
   </si>
@@ -107,9 +107,6 @@
     <t>platform game</t>
   </si>
   <si>
-    <t>3d platformer</t>
-  </si>
-  <si>
     <t>strategy-rpg</t>
   </si>
   <si>
@@ -302,10 +299,121 @@
     <t>tbs</t>
   </si>
   <si>
-    <t>real-time</t>
-  </si>
-  <si>
-    <t>real time</t>
+    <t>real-time strategy</t>
+  </si>
+  <si>
+    <t>real time strategy</t>
+  </si>
+  <si>
+    <t>weapon based fighting</t>
+  </si>
+  <si>
+    <t>2d weapon based fighting</t>
+  </si>
+  <si>
+    <t>weapon-based fighting</t>
+  </si>
+  <si>
+    <t>puzzle &amp; cards</t>
+  </si>
+  <si>
+    <t>puzzle card</t>
+  </si>
+  <si>
+    <t>flight combat</t>
+  </si>
+  <si>
+    <t>aerial combat</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>wargame</t>
+  </si>
+  <si>
+    <t>multiplayer battle arena</t>
+  </si>
+  <si>
+    <t>moba</t>
+  </si>
+  <si>
+    <t>full motion video (fmv)</t>
+  </si>
+  <si>
+    <t>fvm</t>
+  </si>
+  <si>
+    <t>sci-fi puzzle-platform game</t>
+  </si>
+  <si>
+    <t>sci-fi puzzle platform game</t>
+  </si>
+  <si>
+    <t>american football</t>
+  </si>
+  <si>
+    <t>american-football</t>
+  </si>
+  <si>
+    <t>soccer</t>
+  </si>
+  <si>
+    <t>traditional soccer</t>
+  </si>
+  <si>
+    <t>space combat sim</t>
+  </si>
+  <si>
+    <t>space combat simulation</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>3-d</t>
+  </si>
+  <si>
+    <t>augmented reality</t>
+  </si>
+  <si>
+    <t>virtual reality</t>
+  </si>
+  <si>
+    <t>light gun</t>
+  </si>
+  <si>
+    <t>light-gun</t>
+  </si>
+  <si>
+    <t>historic action-adventure</t>
+  </si>
+  <si>
+    <t>historical action adventure</t>
+  </si>
+  <si>
+    <t>third-person action-adventure</t>
+  </si>
+  <si>
+    <t>third-person action adventure</t>
+  </si>
+  <si>
+    <t>run and gun</t>
+  </si>
+  <si>
+    <t>run gun</t>
+  </si>
+  <si>
+    <t>construction and management simulation</t>
+  </si>
+  <si>
+    <t>construction management simulation</t>
+  </si>
+  <si>
+    <t>trivia</t>
+  </si>
+  <si>
+    <t>quiz</t>
   </si>
 </sst>
 </file>
@@ -699,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27B1DF5-292F-4CAE-B96E-0AC01ED929CA}">
-  <dimension ref="A2:F41"/>
+  <dimension ref="A2:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="142" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -765,7 +873,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -789,28 +897,25 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -818,7 +923,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -826,128 +931,128 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -955,15 +1060,15 @@
         <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -984,18 +1089,18 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
         <v>66</v>
-      </c>
-      <c r="B31" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1003,85 +1108,240 @@
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
         <v>82</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
         <v>86</v>
-      </c>
-      <c r="B40" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>89</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>